<commit_message>
Actualización Checklist Auditoría Junio
</commit_message>
<xml_diff>
--- a/qualtcom/Procesos/Calidad/Checklist_Auditoría-150625.xlsx
+++ b/qualtcom/Procesos/Calidad/Checklist_Auditoría-150625.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="132">
   <si>
     <t>DATOS GENERALES</t>
   </si>
@@ -383,9 +383,6 @@
     <t>Fidel Reyna</t>
   </si>
   <si>
-    <t>En proceso</t>
-  </si>
-  <si>
     <t>Cerrada</t>
   </si>
   <si>
@@ -408,6 +405,21 @@
   </si>
   <si>
     <t>Junio 25,2015</t>
+  </si>
+  <si>
+    <t>Junio 29,2015</t>
+  </si>
+  <si>
+    <t>Junio 29 2015</t>
+  </si>
+  <si>
+    <t>Quedó resuelta al marcar el faltante</t>
+  </si>
+  <si>
+    <t>Se realizó el respaldo por equipo en la fecha estipulada</t>
+  </si>
+  <si>
+    <t>Se realizó la limpieza por equipo en la fecha estipulada</t>
   </si>
 </sst>
 </file>
@@ -1304,7 +1316,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -40515,11 +40527,6 @@
     <row r="208" s="31" customFormat="1"/>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C65:F65"/>
-    <mergeCell ref="C75:F75"/>
-    <mergeCell ref="C98:F98"/>
-    <mergeCell ref="C110:F110"/>
-    <mergeCell ref="C126:F126"/>
     <mergeCell ref="C54:F54"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
@@ -40531,6 +40538,11 @@
     <mergeCell ref="C16:F16"/>
     <mergeCell ref="C33:F33"/>
     <mergeCell ref="C46:F46"/>
+    <mergeCell ref="C65:F65"/>
+    <mergeCell ref="C75:F75"/>
+    <mergeCell ref="C98:F98"/>
+    <mergeCell ref="C110:F110"/>
+    <mergeCell ref="C126:F126"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="1.1437007874015748" bottom="1.1437007874015748" header="0.75" footer="0.75"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -41100,6 +41112,12 @@
     <row r="213" s="31" customFormat="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="B4:C4"/>
     <mergeCell ref="C90:F90"/>
     <mergeCell ref="C102:F102"/>
     <mergeCell ref="C118:F118"/>
@@ -41109,12 +41127,6 @@
     <mergeCell ref="C46:F46"/>
     <mergeCell ref="C57:F57"/>
     <mergeCell ref="C67:F67"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="1.1437007874015748" bottom="1.1437007874015748" header="0.75" footer="0.75"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -41126,8 +41138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:H30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -41200,13 +41212,13 @@
         <v>112</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H6" s="45" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="30">
@@ -41214,76 +41226,92 @@
         <v>2</v>
       </c>
       <c r="C7" s="45" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>110</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
-      <c r="F7" s="16"/>
+      <c r="F7" s="16" t="s">
+        <v>127</v>
+      </c>
       <c r="G7" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="H7" s="16"/>
+      <c r="H7" s="45" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="8" spans="2:8" ht="60">
       <c r="B8" s="16">
         <v>3</v>
       </c>
       <c r="C8" s="45" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>110</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
-      <c r="F8" s="16"/>
+      <c r="F8" s="16" t="s">
+        <v>127</v>
+      </c>
       <c r="G8" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="H8" s="16"/>
+      <c r="H8" s="45" t="s">
+        <v>129</v>
+      </c>
     </row>
-    <row r="9" spans="2:8" ht="38.25">
+    <row r="9" spans="2:8" ht="45">
       <c r="B9" s="16">
         <v>4</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D9" s="16" t="s">
         <v>110</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
-      <c r="F9" s="16"/>
+      <c r="F9" s="16" t="s">
+        <v>128</v>
+      </c>
       <c r="G9" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="H9" s="16"/>
+      <c r="H9" s="45" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="10" spans="2:8" ht="63.75">
       <c r="B10" s="16">
         <v>5</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>110</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
-      <c r="F10" s="16"/>
+      <c r="F10" s="16" t="s">
+        <v>128</v>
+      </c>
       <c r="G10" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="H10" s="16"/>
+      <c r="H10" s="45" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="16"/>

</xml_diff>